<commit_message>
Add cards-product block, update importer
Automated migration updates generated by Experience Modernization Agent.

Changed files (8):
- blocks/cards-product/cards-product.css
- styles/styles.css
- tools/importer/import-product-page.bundle.js
- tools/importer/import-product-page.js
- tools/importer/page-templates.json
- tools/importer/reports/import-product-page.report.xlsx
- tools/importer/reports/products/wireless-plans.report.json
- tools/importer/urls-reimport-wireless.txt
</commit_message>
<xml_diff>
--- a/tools/importer/reports/import-product-page.report.xlsx
+++ b/tools/importer/reports/import-product-page.report.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="163">
   <si>
     <t>_reportFile</t>
   </si>
@@ -61,6 +61,240 @@
     <t>https://www.business.att.com/</t>
   </si>
   <si>
+    <t>learn.report.json</t>
+  </si>
+  <si>
+    <t>["hero-banner","cards-story","cards-story"]</t>
+  </si>
+  <si>
+    <t>learn</t>
+  </si>
+  <si>
+    <t>hub-page</t>
+  </si>
+  <si>
+    <t>2026-03-02T10:02:52.172Z</t>
+  </si>
+  <si>
+    <t>Welcome To Business Insights and Technology Advice</t>
+  </si>
+  <si>
+    <t>https://www.business.att.com/learn.html</t>
+  </si>
+  <si>
+    <t>small-business.report.json</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>small-business</t>
+  </si>
+  <si>
+    <t>industry-page</t>
+  </si>
+  <si>
+    <t>2026-03-02T10:02:14.236Z</t>
+  </si>
+  <si>
+    <t>Explore AT&amp;T Internet Devices for Home and Small Business</t>
+  </si>
+  <si>
+    <t>https://www.business.att.com/small-business.html</t>
+  </si>
+  <si>
+    <t>support.report.json</t>
+  </si>
+  <si>
+    <t>support</t>
+  </si>
+  <si>
+    <t>2026-03-02T10:03:04.405Z</t>
+  </si>
+  <si>
+    <t>AT&amp;T Business Support</t>
+  </si>
+  <si>
+    <t>https://www.business.att.com/support.html</t>
+  </si>
+  <si>
+    <t>about/why-att-business.report.json</t>
+  </si>
+  <si>
+    <t>["hero-banner","cards-value","columns-offer","accordion-links"]</t>
+  </si>
+  <si>
+    <t>about/why-att-business</t>
+  </si>
+  <si>
+    <t>landing-page</t>
+  </si>
+  <si>
+    <t>2026-03-02T10:02:29.654Z</t>
+  </si>
+  <si>
+    <t>Why Customers Choose AT&amp;T Business For Expert Guidance and Advice</t>
+  </si>
+  <si>
+    <t>https://www.business.att.com/about/why-att-business.html</t>
+  </si>
+  <si>
+    <t>industries/finance.report.json</t>
+  </si>
+  <si>
+    <t>["hero-banner","hero-banner"]</t>
+  </si>
+  <si>
+    <t>industries/finance</t>
+  </si>
+  <si>
+    <t>2026-03-02T10:01:49.111Z</t>
+  </si>
+  <si>
+    <t>Financial Technology &amp; Security Solutions at AT&amp;T Business.</t>
+  </si>
+  <si>
+    <t>https://www.business.att.com/industries/finance.html</t>
+  </si>
+  <si>
+    <t>industries/healthcare.report.json</t>
+  </si>
+  <si>
+    <t>["hero-banner","cards-value","columns-offer"]</t>
+  </si>
+  <si>
+    <t>industries/healthcare</t>
+  </si>
+  <si>
+    <t>2026-03-02T10:01:33.523Z</t>
+  </si>
+  <si>
+    <t>Cybersecurity, Networking &amp; Iot Healthcare Solutions at AT&amp;T.</t>
+  </si>
+  <si>
+    <t>https://www.business.att.com/industries/healthcare.html</t>
+  </si>
+  <si>
+    <t>industries/hospitality.report.json</t>
+  </si>
+  <si>
+    <t>["hero-banner","hero-banner","columns-offer"]</t>
+  </si>
+  <si>
+    <t>industries/hospitality</t>
+  </si>
+  <si>
+    <t>2026-03-02T10:01:43.957Z</t>
+  </si>
+  <si>
+    <t>Hospitality Technology &amp; Guest Service Solutions at AT&amp;T Business.</t>
+  </si>
+  <si>
+    <t>https://www.business.att.com/industries/hospitality.html</t>
+  </si>
+  <si>
+    <t>industries/manufacturing.report.json</t>
+  </si>
+  <si>
+    <t>["hero-banner","cards-value","columns-offer","columns-offer","columns-offer"]</t>
+  </si>
+  <si>
+    <t>industries/manufacturing</t>
+  </si>
+  <si>
+    <t>2026-03-02T10:02:00.717Z</t>
+  </si>
+  <si>
+    <t>IOT Network and Technology Solutions for Manufactures at AT&amp;T Business</t>
+  </si>
+  <si>
+    <t>https://www.business.att.com/industries/manufacturing.html</t>
+  </si>
+  <si>
+    <t>industries/public-sector.report.json</t>
+  </si>
+  <si>
+    <t>["hero-banner","hero-banner","hero-banner","hero-banner","columns-offer","columns-offer"]</t>
+  </si>
+  <si>
+    <t>industries/public-sector</t>
+  </si>
+  <si>
+    <t>2026-03-02T10:02:08.188Z</t>
+  </si>
+  <si>
+    <t>AT&amp;T Public Sector Solutions deliver a faster, smarter, safer future</t>
+  </si>
+  <si>
+    <t>https://www.business.att.com/industries/public-sector.html</t>
+  </si>
+  <si>
+    <t>industries/retail.report.json</t>
+  </si>
+  <si>
+    <t>industries/retail</t>
+  </si>
+  <si>
+    <t>2026-03-02T10:01:39.311Z</t>
+  </si>
+  <si>
+    <t>Connected Consumer &amp; Retail Technology Solutions at AT&amp;T Business.</t>
+  </si>
+  <si>
+    <t>https://www.business.att.com/industries/retail.html</t>
+  </si>
+  <si>
+    <t>industries/transportation.report.json</t>
+  </si>
+  <si>
+    <t>industries/transportation</t>
+  </si>
+  <si>
+    <t>2026-03-02T10:01:53.480Z</t>
+  </si>
+  <si>
+    <t>Fiber, 5G and other digital solutions for the transportation industry</t>
+  </si>
+  <si>
+    <t>https://www.business.att.com/industries/transportation.html</t>
+  </si>
+  <si>
+    <t>learn/customer-stories.report.json</t>
+  </si>
+  <si>
+    <t>["hero-banner"]</t>
+  </si>
+  <si>
+    <t>learn/customer-stories</t>
+  </si>
+  <si>
+    <t>2026-03-02T10:02:58.245Z</t>
+  </si>
+  <si>
+    <t>Customer Stories | AT&amp;T Business</t>
+  </si>
+  <si>
+    <t>https://www.business.att.com/learn/customer-stories.html</t>
+  </si>
+  <si>
+    <t>offers/switch-to-att-business.report.json</t>
+  </si>
+  <si>
+    <t>["hero-banner","cards-value","cards-value","cards-product","columns-offer"]</t>
+  </si>
+  <si>
+    <t>offers/switch-to-att-business</t>
+  </si>
+  <si>
+    <t>2026-03-02T10:02:36.674Z</t>
+  </si>
+  <si>
+    <t>Change your wireless carrier and internet. Switch to AT&amp;T Business</t>
+  </si>
+  <si>
+    <t>https://www.business.att.com/offers/switch-to-att-business.html</t>
+  </si>
+  <si>
     <t>portfolios/business-internet.report.json</t>
   </si>
   <si>
@@ -232,19 +466,40 @@
     <t>products/wireless-plans.report.json</t>
   </si>
   <si>
-    <t>["columns-offer","accordion-faq"]</t>
+    <t>["hero-banner","cards-product","cards-product","cards-product","cards-value","cards-value","hero-dark","hero-dark","hero-dark","columns-offer","accordion-faq"]</t>
   </si>
   <si>
     <t>products/wireless-plans</t>
   </si>
   <si>
-    <t>2026-03-02T10:00:59.653Z</t>
+    <t>2026-03-02T13:40:12.511Z</t>
   </si>
   <si>
     <t>Business Cell Phone Plans | AT&amp;T Business Wireless &amp; Mobile</t>
   </si>
   <si>
     <t>https://www.business.att.com/products/wireless-plans.html</t>
+  </si>
+  <si>
+    <t>learn/customer-stories/parkville.report.json</t>
+  </si>
+  <si>
+    <t>["cards-value","cards-promo","columns-offer"]</t>
+  </si>
+  <si>
+    <t>learn/customer-stories/parkville</t>
+  </si>
+  <si>
+    <t>customer-story</t>
+  </si>
+  <si>
+    <t>2026-03-02T10:03:23.971Z</t>
+  </si>
+  <si>
+    <t>Parkville Creekside Development Relies on AT&amp;T Business Fiber</t>
+  </si>
+  <si>
+    <t>https://www.business.att.com/learn/customer-stories/parkville.html</t>
   </si>
 </sst>
 </file>
@@ -633,7 +888,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -742,24 +997,24 @@
         <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="F4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
         <v>31</v>
@@ -794,85 +1049,85 @@
         <v>11</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="F6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D7" t="s">
         <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="F7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D8" t="s">
         <v>11</v>
       </c>
       <c r="E8" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="F8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G8" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H8" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
       </c>
       <c r="E9" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="F9" t="s">
         <v>57</v>
@@ -898,7 +1153,7 @@
         <v>11</v>
       </c>
       <c r="E10" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="F10" t="s">
         <v>63</v>
@@ -924,7 +1179,7 @@
         <v>11</v>
       </c>
       <c r="E11" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="F11" t="s">
         <v>69</v>
@@ -941,25 +1196,389 @@
         <v>72</v>
       </c>
       <c r="B12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" t="s">
         <v>73</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" t="s">
         <v>74</v>
       </c>
-      <c r="D12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" t="s">
-        <v>56</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>75</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>76</v>
       </c>
-      <c r="H12" t="s">
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>77</v>
+      </c>
+      <c r="B13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" t="s">
+        <v>78</v>
+      </c>
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" t="s">
+        <v>79</v>
+      </c>
+      <c r="G13" t="s">
+        <v>80</v>
+      </c>
+      <c r="H13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14" t="s">
+        <v>83</v>
+      </c>
+      <c r="C14" t="s">
+        <v>84</v>
+      </c>
+      <c r="D14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" t="s">
+        <v>85</v>
+      </c>
+      <c r="G14" t="s">
+        <v>86</v>
+      </c>
+      <c r="H14" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>88</v>
+      </c>
+      <c r="B15" t="s">
+        <v>89</v>
+      </c>
+      <c r="C15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" t="s">
+        <v>91</v>
+      </c>
+      <c r="G15" t="s">
+        <v>92</v>
+      </c>
+      <c r="H15" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>94</v>
+      </c>
+      <c r="B16" t="s">
+        <v>95</v>
+      </c>
+      <c r="C16" t="s">
+        <v>96</v>
+      </c>
+      <c r="D16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" t="s">
+        <v>97</v>
+      </c>
+      <c r="F16" t="s">
+        <v>98</v>
+      </c>
+      <c r="G16" t="s">
+        <v>99</v>
+      </c>
+      <c r="H16" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>101</v>
+      </c>
+      <c r="B17" t="s">
+        <v>102</v>
+      </c>
+      <c r="C17" t="s">
+        <v>103</v>
+      </c>
+      <c r="D17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" t="s">
+        <v>97</v>
+      </c>
+      <c r="F17" t="s">
+        <v>104</v>
+      </c>
+      <c r="G17" t="s">
+        <v>105</v>
+      </c>
+      <c r="H17" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>107</v>
+      </c>
+      <c r="B18" t="s">
+        <v>108</v>
+      </c>
+      <c r="C18" t="s">
+        <v>109</v>
+      </c>
+      <c r="D18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" t="s">
+        <v>97</v>
+      </c>
+      <c r="F18" t="s">
+        <v>110</v>
+      </c>
+      <c r="G18" t="s">
+        <v>111</v>
+      </c>
+      <c r="H18" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>113</v>
+      </c>
+      <c r="B19" t="s">
+        <v>114</v>
+      </c>
+      <c r="C19" t="s">
+        <v>115</v>
+      </c>
+      <c r="D19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" t="s">
+        <v>97</v>
+      </c>
+      <c r="F19" t="s">
+        <v>116</v>
+      </c>
+      <c r="G19" t="s">
+        <v>117</v>
+      </c>
+      <c r="H19" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>119</v>
+      </c>
+      <c r="B20" t="s">
+        <v>120</v>
+      </c>
+      <c r="C20" t="s">
+        <v>121</v>
+      </c>
+      <c r="D20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" t="s">
+        <v>97</v>
+      </c>
+      <c r="F20" t="s">
+        <v>122</v>
+      </c>
+      <c r="G20" t="s">
+        <v>123</v>
+      </c>
+      <c r="H20" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>125</v>
+      </c>
+      <c r="B21" t="s">
+        <v>126</v>
+      </c>
+      <c r="C21" t="s">
+        <v>127</v>
+      </c>
+      <c r="D21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" t="s">
+        <v>97</v>
+      </c>
+      <c r="F21" t="s">
+        <v>128</v>
+      </c>
+      <c r="G21" t="s">
+        <v>129</v>
+      </c>
+      <c r="H21" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>131</v>
+      </c>
+      <c r="B22" t="s">
+        <v>132</v>
+      </c>
+      <c r="C22" t="s">
+        <v>133</v>
+      </c>
+      <c r="D22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" t="s">
+        <v>134</v>
+      </c>
+      <c r="F22" t="s">
+        <v>135</v>
+      </c>
+      <c r="G22" t="s">
+        <v>136</v>
+      </c>
+      <c r="H22" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>138</v>
+      </c>
+      <c r="B23" t="s">
+        <v>139</v>
+      </c>
+      <c r="C23" t="s">
+        <v>140</v>
+      </c>
+      <c r="D23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" t="s">
+        <v>134</v>
+      </c>
+      <c r="F23" t="s">
+        <v>141</v>
+      </c>
+      <c r="G23" t="s">
+        <v>142</v>
+      </c>
+      <c r="H23" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>144</v>
+      </c>
+      <c r="B24" t="s">
+        <v>145</v>
+      </c>
+      <c r="C24" t="s">
+        <v>146</v>
+      </c>
+      <c r="D24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" t="s">
+        <v>134</v>
+      </c>
+      <c r="F24" t="s">
+        <v>147</v>
+      </c>
+      <c r="G24" t="s">
+        <v>148</v>
+      </c>
+      <c r="H24" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>150</v>
+      </c>
+      <c r="B25" t="s">
+        <v>151</v>
+      </c>
+      <c r="C25" t="s">
+        <v>152</v>
+      </c>
+      <c r="D25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" t="s">
+        <v>134</v>
+      </c>
+      <c r="F25" t="s">
+        <v>153</v>
+      </c>
+      <c r="G25" t="s">
+        <v>154</v>
+      </c>
+      <c r="H25" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>156</v>
+      </c>
+      <c r="B26" t="s">
+        <v>157</v>
+      </c>
+      <c r="C26" t="s">
+        <v>158</v>
+      </c>
+      <c r="D26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" t="s">
+        <v>159</v>
+      </c>
+      <c r="F26" t="s">
+        <v>160</v>
+      </c>
+      <c r="G26" t="s">
+        <v>161</v>
+      </c>
+      <c r="H26" t="s">
+        <v>162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>